<commit_message>
MS: additional unit tests; providing basic CellStyle functionality
git-svn-id: svn://ms72.weblink.ch/mirai/XLConnect-R@40 ccc6e944-403e-a54a-b5f3-c2babcd103ea
</commit_message>
<xml_diff>
--- a/inst/unitTests/resources/testWorkbookDefinedNames.xlsx
+++ b/inst/unitTests/resources/testWorkbookDefinedNames.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17730" windowHeight="7305" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="First Sheet" sheetId="1" r:id="rId1"/>
@@ -16,9 +16,10 @@
     <definedName name="FirstName">'Third Sheet'!$C$5:$D$7</definedName>
     <definedName name="FourthName">'Second Sheet'!$E$12</definedName>
     <definedName name="SecondName">'Third Sheet'!$K$15:$P$15</definedName>
-    <definedName name="ThirdName">'First Sheet'!$E$12:$G$16</definedName>
+    <definedName name="ThirdName">#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1:N22"/>
 </workbook>
 </file>
 
@@ -580,7 +581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -600,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C5:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>